<commit_message>
aggiornata checklist, data.json e folder FILES
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/accreditamento-checklist_V8.2.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS 1.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9AD02D-6902-48F2-AEFD-CA892F65E731}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67716826-FE16-476A-8A09-52F36A6FDB7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1731,12 +1731,6 @@
     <t>2.16.840.1.113883.2.9.2.30.4.4.467ffdcd304925eefdbefe1090e5ac75d679495c7e3561c8f0d3a0514d37260c.54f2499907^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-01-29T14:17:57Z</t>
-  </si>
-  <si>
-    <t>1373d9a6af7044db</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -1755,12 +1749,6 @@
 In conclusione, è l'applicativo che, a priori, compila i valori del JWT e il PLS non ha nessun tipo di accesso alla sua compilazione.</t>
   </si>
   <si>
-    <t>2024-01-29T14:24:14Z</t>
-  </si>
-  <si>
-    <t>fae42361425536ee</t>
-  </si>
-  <si>
     <t>Il PLS viene avvisato con l'errore mostrato a video e viene annullato l'invio del PS.
 Il test è stato effettuato per completezza e per mostrarvi l'eventuale finestra di dialogo che viene mostrata al medico in caso di errore.
 Per quanto riguarda questo specifico test non c'è possibilità da parte del medico di modificare il contenuto dei campi presenti nel token che vengono demandati completamente all'applicativo nella sua compilazione.
@@ -1773,15 +1761,6 @@
 "Se il problema dovesse persistere contattere l'help desk di Junior Bit."</t>
   </si>
   <si>
-    <t>2023-11-09T12:01:01Z</t>
-  </si>
-  <si>
-    <t>259d37d522348629</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.442cad0d64820a099ee7d33aad276c1f1bd4920047942c752dded4917b27f7d3.c2c25144bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Essendo comunque una sezione obbligatoria, non c'è modo che il medico possa omettere questa sezione nel compilare il CDA</t>
   </si>
   <si>
@@ -1811,6 +1790,27 @@
 Il CDA e il token JWT sono generati dinamicamente all'interno della stessa scheda del paziente per cui il PLS ha deciso di redigere il PSS e sottoporlo al processo di validazione.
 Di conseguenza utilizzando in input la stessa fonte non c'è possibilità da parte del PLS (e del conseguente invio verso i servizi di validazione) che vengano inseriti due CF differenti.
 Il test è stato effettuato per mostrare a video eventuali errori e come vengono segnalati al medico.</t>
+  </si>
+  <si>
+    <t>73f9ccd6843d14fd5eb38a731d880065</t>
+  </si>
+  <si>
+    <t>2026-02-10T12:12:50Z</t>
+  </si>
+  <si>
+    <t>2bd81b8ad6606022675b0dbfd4bc49d8</t>
+  </si>
+  <si>
+    <t>2026-02-10T12:18:47Z</t>
+  </si>
+  <si>
+    <t>8ad4a3edb79ef22fdd44fda84daf1b87</t>
+  </si>
+  <si>
+    <t>2026-02-10T12:27:05Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.f3cd68ef8cad77c24af64f13ceb67704fd7984c39df367465f3f36e50aa2d7ef.7ce5c1affe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3957,10 +3957,10 @@
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A131" sqref="A131:XFD131"/>
+      <selection pane="bottomRight" activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4375,16 +4375,16 @@
         <v>43</v>
       </c>
       <c r="F13" s="57">
-        <v>45320</v>
+        <v>46063</v>
       </c>
       <c r="G13" s="58" t="s">
+        <v>464</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>463</v>
+      </c>
+      <c r="I13" s="58" t="s">
         <v>446</v>
-      </c>
-      <c r="H13" s="58" t="s">
-        <v>447</v>
-      </c>
-      <c r="I13" s="58" t="s">
-        <v>448</v>
       </c>
       <c r="J13" s="38" t="s">
         <v>64</v>
@@ -4398,7 +4398,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="P13" s="38" t="s">
         <v>226</v>
@@ -4406,7 +4406,7 @@
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="T13" s="38"/>
       <c r="U13" s="39"/>
@@ -4445,7 +4445,7 @@
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
       <c r="S14" s="38" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="T14" s="38"/>
       <c r="U14" s="39"/>
@@ -4484,7 +4484,7 @@
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="38" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="T15" s="38"/>
       <c r="U15" s="39"/>
@@ -4523,7 +4523,7 @@
       <c r="Q16" s="38"/>
       <c r="R16" s="38"/>
       <c r="S16" s="38" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T16" s="38"/>
       <c r="U16" s="39"/>
@@ -4697,16 +4697,16 @@
         <v>55</v>
       </c>
       <c r="F21" s="57">
-        <v>45320</v>
+        <v>46063</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="H21" s="58" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="I21" s="58" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J21" s="38" t="s">
         <v>64</v>
@@ -4720,7 +4720,7 @@
         <v>64</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="P21" s="38" t="s">
         <v>226</v>
@@ -4728,7 +4728,7 @@
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
       <c r="S21" s="38" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="T21" s="38"/>
       <c r="U21" s="39"/>
@@ -5032,7 +5032,7 @@
         <v>64</v>
       </c>
       <c r="O29" s="38" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="P29" s="38" t="s">
         <v>226</v>
@@ -5044,7 +5044,7 @@
         <v>226</v>
       </c>
       <c r="S29" s="38" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="T29" s="38"/>
       <c r="U29" s="39" t="s">
@@ -8819,16 +8819,16 @@
         <v>333</v>
       </c>
       <c r="F131" s="57">
-        <v>45239</v>
+        <v>46063</v>
       </c>
       <c r="G131" s="58" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="H131" s="58" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="I131" s="58" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="J131" s="38" t="s">
         <v>64</v>
@@ -8842,7 +8842,7 @@
         <v>64</v>
       </c>
       <c r="O131" s="38" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="P131" s="38" t="s">
         <v>226</v>
@@ -8854,7 +8854,7 @@
         <v>226</v>
       </c>
       <c r="S131" s="38" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="T131" s="38"/>
       <c r="U131" s="39"/>
@@ -9054,7 +9054,7 @@
         <v>235</v>
       </c>
       <c r="L136" s="38" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="M136" s="38"/>
       <c r="N136" s="38"/>
@@ -9097,7 +9097,7 @@
         <v>235</v>
       </c>
       <c r="L137" s="38" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="M137" s="38"/>
       <c r="N137" s="38"/>
@@ -9140,7 +9140,7 @@
         <v>235</v>
       </c>
       <c r="L138" s="38" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="M138" s="38"/>
       <c r="N138" s="38"/>
@@ -11139,7 +11139,7 @@
         <v>235</v>
       </c>
       <c r="L191" s="50" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="M191" s="50"/>
       <c r="N191" s="50"/>
@@ -11182,7 +11182,7 @@
         <v>235</v>
       </c>
       <c r="L192" s="50" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="M192" s="50"/>
       <c r="N192" s="50"/>
@@ -17492,21 +17492,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -17650,32 +17635,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17693,6 +17668,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>